<commit_message>
Update folders to move
</commit_message>
<xml_diff>
--- a/xftomaui/NameMappings.xlsx
+++ b/xftomaui/NameMappings.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\code\xf-to-maui\xftomaui\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B4DBCDB-95FC-4230-89C2-1BB777BB37D5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7318A6E7-DB42-4634-9AF9-0847E2DA859C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2844" yWindow="1464" windowWidth="19548" windowHeight="14664" xr2:uid="{AB42A6E3-4848-A147-B598-85F847833A81}"/>
+    <workbookView xWindow="5400" yWindow="1224" windowWidth="34332" windowHeight="14664" activeTab="4" xr2:uid="{AB42A6E3-4848-A147-B598-85F847833A81}"/>
   </bookViews>
   <sheets>
     <sheet name="Maui.Essentials" sheetId="1" r:id="rId1"/>
@@ -20,6 +20,9 @@
     <sheet name="Directories" sheetId="5" r:id="rId5"/>
     <sheet name="Files" sheetId="6" r:id="rId6"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">Directories!$A$1:$B$42</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -39,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="424" uniqueCount="412">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="426" uniqueCount="414">
   <si>
     <t>Xamarin.Platform.Handlers.DeviceTests.Handlers.Layout</t>
   </si>
@@ -1275,6 +1278,12 @@
   </si>
   <si>
     <t>New Filename</t>
+  </si>
+  <si>
+    <t>./src/Platform.Handlers/samples</t>
+  </si>
+  <si>
+    <t>./src/Handlers/samples</t>
   </si>
 </sst>
 </file>
@@ -1646,7 +1655,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C5380A5-EC7E-1945-9F1A-CCCFB8EF0089}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
@@ -2552,10 +2561,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0873AE8A-7AB4-EC41-9198-123A3D96031C}">
-  <dimension ref="A1:B42"/>
+  <dimension ref="A1:B43"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="C28" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -2573,333 +2582,346 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>126</v>
+        <v>132</v>
       </c>
       <c r="B2" t="s">
-        <v>110</v>
+        <v>322</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>153</v>
+        <v>135</v>
       </c>
       <c r="B3" t="s">
-        <v>125</v>
+        <v>323</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>152</v>
+        <v>131</v>
       </c>
       <c r="B4" t="s">
-        <v>124</v>
+        <v>324</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>147</v>
+        <v>134</v>
       </c>
       <c r="B5" t="s">
-        <v>310</v>
+        <v>325</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>148</v>
+        <v>136</v>
       </c>
       <c r="B6" t="s">
-        <v>311</v>
+        <v>321</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="B7" t="s">
-        <v>312</v>
+        <v>326</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>145</v>
+        <v>133</v>
       </c>
       <c r="B8" t="s">
-        <v>313</v>
+        <v>327</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>146</v>
+        <v>130</v>
       </c>
       <c r="B9" t="s">
-        <v>314</v>
+        <v>328</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="B10" t="s">
-        <v>315</v>
+        <v>329</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B11" t="s">
-        <v>316</v>
+        <v>330</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="B12" t="s">
-        <v>317</v>
+        <v>331</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>149</v>
+        <v>127</v>
       </c>
       <c r="B13" t="s">
-        <v>318</v>
+        <v>332</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>150</v>
+        <v>129</v>
       </c>
       <c r="B14" t="s">
-        <v>319</v>
+        <v>333</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>151</v>
+        <v>128</v>
       </c>
       <c r="B15" t="s">
-        <v>320</v>
+        <v>334</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>121</v>
+        <v>147</v>
       </c>
       <c r="B16" t="s">
-        <v>162</v>
+        <v>310</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>123</v>
+        <v>148</v>
       </c>
       <c r="B17" t="s">
-        <v>154</v>
+        <v>311</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>122</v>
+        <v>143</v>
       </c>
       <c r="B18" t="s">
-        <v>157</v>
+        <v>312</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>120</v>
+        <v>145</v>
       </c>
       <c r="B19" t="s">
-        <v>155</v>
+        <v>313</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>119</v>
+        <v>146</v>
       </c>
       <c r="B20" t="s">
-        <v>156</v>
+        <v>314</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>118</v>
+        <v>142</v>
       </c>
       <c r="B21" t="s">
-        <v>158</v>
+        <v>315</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>116</v>
+        <v>141</v>
       </c>
       <c r="B22" t="s">
-        <v>159</v>
+        <v>316</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>117</v>
+        <v>144</v>
       </c>
       <c r="B23" t="s">
-        <v>160</v>
+        <v>317</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>115</v>
+        <v>149</v>
       </c>
       <c r="B24" t="s">
-        <v>161</v>
+        <v>318</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>113</v>
+        <v>150</v>
       </c>
       <c r="B25" t="s">
-        <v>163</v>
+        <v>319</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>114</v>
+        <v>151</v>
       </c>
       <c r="B26" t="s">
-        <v>164</v>
+        <v>320</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>112</v>
+        <v>121</v>
       </c>
       <c r="B27" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>111</v>
+        <v>122</v>
       </c>
       <c r="B28" t="s">
-        <v>166</v>
+        <v>157</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>136</v>
+        <v>123</v>
       </c>
       <c r="B29" t="s">
-        <v>321</v>
+        <v>154</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>132</v>
+        <v>118</v>
       </c>
       <c r="B30" t="s">
-        <v>322</v>
+        <v>158</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>135</v>
+        <v>116</v>
       </c>
       <c r="B31" t="s">
-        <v>323</v>
+        <v>159</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>131</v>
+        <v>153</v>
       </c>
       <c r="B32" t="s">
-        <v>324</v>
+        <v>125</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>134</v>
+        <v>152</v>
       </c>
       <c r="B33" t="s">
-        <v>325</v>
+        <v>124</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>137</v>
+        <v>119</v>
       </c>
       <c r="B34" t="s">
-        <v>326</v>
+        <v>156</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>133</v>
+        <v>120</v>
       </c>
       <c r="B35" t="s">
-        <v>327</v>
+        <v>155</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>130</v>
+        <v>117</v>
       </c>
       <c r="B36" t="s">
-        <v>328</v>
+        <v>160</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>138</v>
+        <v>126</v>
       </c>
       <c r="B37" t="s">
-        <v>329</v>
+        <v>110</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>140</v>
+        <v>115</v>
       </c>
       <c r="B38" t="s">
-        <v>330</v>
+        <v>161</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>139</v>
+        <v>113</v>
       </c>
       <c r="B39" t="s">
-        <v>331</v>
+        <v>163</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>127</v>
+        <v>114</v>
       </c>
       <c r="B40" t="s">
-        <v>332</v>
+        <v>164</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>129</v>
+        <v>112</v>
       </c>
       <c r="B41" t="s">
-        <v>333</v>
+        <v>165</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>128</v>
+        <v>111</v>
       </c>
       <c r="B42" t="s">
-        <v>334</v>
+        <v>166</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>412</v>
+      </c>
+      <c r="B43" t="s">
+        <v>413</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:B42" xr:uid="{C05903AB-6806-4339-983D-A9948E9C764D}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B42">
+      <sortCondition ref="B1:B42"/>
+    </sortState>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -2908,7 +2930,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57691AD4-EC7F-314E-AE2B-7AE44975FF17}">
   <dimension ref="A1:B66"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A19" workbookViewId="0">
       <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Fix up mappings ordering
</commit_message>
<xml_diff>
--- a/xftomaui/NameMappings.xlsx
+++ b/xftomaui/NameMappings.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\code\xf-to-maui\xftomaui\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7318A6E7-DB42-4634-9AF9-0847E2DA859C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C41D8F02-DAC6-42B5-BAE9-5197683E67CD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5400" yWindow="1224" windowWidth="34332" windowHeight="14664" activeTab="4" xr2:uid="{AB42A6E3-4848-A147-B598-85F847833A81}"/>
+    <workbookView xWindow="4608" yWindow="1176" windowWidth="20916" windowHeight="14664" activeTab="4" xr2:uid="{AB42A6E3-4848-A147-B598-85F847833A81}"/>
   </bookViews>
   <sheets>
     <sheet name="Maui.Essentials" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="426" uniqueCount="414">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="434" uniqueCount="422">
   <si>
     <t>Xamarin.Platform.Handlers.DeviceTests.Handlers.Layout</t>
   </si>
@@ -1284,6 +1284,30 @@
   </si>
   <si>
     <t>./src/Handlers/samples</t>
+  </si>
+  <si>
+    <t>Xamarin.Essentials.sln</t>
+  </si>
+  <si>
+    <t>Microsoft.Maui.Essentials.sln</t>
+  </si>
+  <si>
+    <t>Xamarin.Forms.ControlGallery.sln</t>
+  </si>
+  <si>
+    <t>ControlGallery.sln</t>
+  </si>
+  <si>
+    <t>Xamarin.Forms.sln</t>
+  </si>
+  <si>
+    <t>Microsoft.Maui.sln</t>
+  </si>
+  <si>
+    <t>Maui.sln</t>
+  </si>
+  <si>
+    <t>Microsoft.Maui-net6.sln</t>
   </si>
 </sst>
 </file>
@@ -2563,8 +2587,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0873AE8A-7AB4-EC41-9198-123A3D96031C}">
   <dimension ref="A1:B43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="C28" sqref="C1:C1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -2582,90 +2606,90 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="B2" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="B3" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="B4" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="B5" t="s">
-        <v>325</v>
+        <v>321</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="B6" t="s">
-        <v>321</v>
+        <v>326</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="B7" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="B8" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>130</v>
+        <v>138</v>
       </c>
       <c r="B9" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="B10" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B11" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>139</v>
+        <v>132</v>
       </c>
       <c r="B12" t="s">
-        <v>331</v>
+        <v>322</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
@@ -2694,66 +2718,66 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="B16" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="B17" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="B18" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="B19" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="B20" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B21" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="B22" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
       <c r="B23" t="s">
-        <v>317</v>
+        <v>310</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
@@ -2928,10 +2952,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57691AD4-EC7F-314E-AE2B-7AE44975FF17}">
-  <dimension ref="A1:B66"/>
+  <dimension ref="A1:B70"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+    <sheetView topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="A72" sqref="A72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -3467,6 +3491,38 @@
         <v>365</v>
       </c>
     </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A67" t="s">
+        <v>414</v>
+      </c>
+      <c r="B67" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A68" t="s">
+        <v>416</v>
+      </c>
+      <c r="B68" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A69" t="s">
+        <v>418</v>
+      </c>
+      <c r="B69" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A70" t="s">
+        <v>420</v>
+      </c>
+      <c r="B70" t="s">
+        <v>421</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Add assembly and rootnamespace mappings
</commit_message>
<xml_diff>
--- a/xftomaui/NameMappings.xlsx
+++ b/xftomaui/NameMappings.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\code\xf-to-maui\xftomaui\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B4F24A4-71B9-4989-8329-1E8B13956F65}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACC74B2B-B056-4919-8F75-349BD8B09DDB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7608" yWindow="2016" windowWidth="20916" windowHeight="14664" activeTab="5" xr2:uid="{AB42A6E3-4848-A147-B598-85F847833A81}"/>
+    <workbookView xWindow="5580" yWindow="1692" windowWidth="20916" windowHeight="14664" firstSheet="2" activeTab="7" xr2:uid="{AB42A6E3-4848-A147-B598-85F847833A81}"/>
   </bookViews>
   <sheets>
     <sheet name="Maui.Essentials" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,8 @@
     <sheet name="Maui.Compatibility" sheetId="4" r:id="rId4"/>
     <sheet name="Directories" sheetId="5" r:id="rId5"/>
     <sheet name="Files" sheetId="6" r:id="rId6"/>
+    <sheet name="RootNamespace" sheetId="7" r:id="rId7"/>
+    <sheet name="AssemblyName" sheetId="8" r:id="rId8"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">Directories!$A$1:$B$42</definedName>
@@ -42,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="432" uniqueCount="420">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="534" uniqueCount="455">
   <si>
     <t>Xamarin.Platform.Handlers.DeviceTests.Handlers.Layout</t>
   </si>
@@ -1302,6 +1304,111 @@
   </si>
   <si>
     <t>Microsoft.Maui.sln</t>
+  </si>
+  <si>
+    <t>Microsoft.Maui.Controls.Flex</t>
+  </si>
+  <si>
+    <t>Xamarin.Forms.Maps.iOS</t>
+  </si>
+  <si>
+    <t>Xamarin.Forms.Maps.MacOS</t>
+  </si>
+  <si>
+    <t>Microsoft.Maui.Controls.Compatibility.Android</t>
+  </si>
+  <si>
+    <t>Microsoft.Maui.Controls.Compatibility.GTK</t>
+  </si>
+  <si>
+    <t>Microsoft.Maui.Controls.Compatibility.iOS</t>
+  </si>
+  <si>
+    <t>Microsoft.Maui.Controls.Compatibility.macOS</t>
+  </si>
+  <si>
+    <t>Microsoft.Maui.Controls.Compatibility.UAP</t>
+  </si>
+  <si>
+    <t>Microsoft.Maui.Controls.GTK</t>
+  </si>
+  <si>
+    <t>Microsoft.Maui.Controls.iOS</t>
+  </si>
+  <si>
+    <t>Microsoft.Maui.Controls.MacOS</t>
+  </si>
+  <si>
+    <t>Microsoft.Maui.Controls.UWP</t>
+  </si>
+  <si>
+    <t>Microsoft.Maui.Controls.Compatibility.Android.AppLinks</t>
+  </si>
+  <si>
+    <t>Microsoft.Maui.Controls.Compatibility.Android.UnitTests</t>
+  </si>
+  <si>
+    <t>Microsoft.Maui.Controls.Compatibility.iOS.UnitTests</t>
+  </si>
+  <si>
+    <t>Microsoft.Maui.Controls.Compatibility.UAP.UnitTests</t>
+  </si>
+  <si>
+    <t>Microsoft.Maui.Handlers.DeviceTests</t>
+  </si>
+  <si>
+    <t>XamarinEssentialsTests</t>
+  </si>
+  <si>
+    <t>EssentialsTests</t>
+  </si>
+  <si>
+    <t>Xamarin.Forms.Maps.macOS</t>
+  </si>
+  <si>
+    <t>Xamarin.Forms.Material</t>
+  </si>
+  <si>
+    <t>XamarinEssentialsDeviceTestsiOS</t>
+  </si>
+  <si>
+    <t>XamarinEssentialsDeviceTestsAndroid</t>
+  </si>
+  <si>
+    <t>XamarinEssentialsDeviceTestsShared</t>
+  </si>
+  <si>
+    <t>XamarinEssentialsDeviceTestsUWP</t>
+  </si>
+  <si>
+    <t>Microsoft.Maui.Controls.Compatibility.Material</t>
+  </si>
+  <si>
+    <t>EssentialsDeviceTestsiOS</t>
+  </si>
+  <si>
+    <t>EssentialsDeviceTestsAndroid</t>
+  </si>
+  <si>
+    <t>EssentialsDeviceTestsShared</t>
+  </si>
+  <si>
+    <t>EssentialsDeviceTestsUWP</t>
+  </si>
+  <si>
+    <t>Microsoft.Maui.Controls.Maps.Android</t>
+  </si>
+  <si>
+    <t>Microsoft.Maui.Controls.Maps.GTK</t>
+  </si>
+  <si>
+    <t>Microsoft.Maui.Controls.Maps.iOS</t>
+  </si>
+  <si>
+    <t>Microsoft.Maui.Controls.Maps.macOS</t>
+  </si>
+  <si>
+    <t>Microsoft.Maui.Controls.Maps.UWP</t>
   </si>
 </sst>
 </file>
@@ -1708,8 +1815,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4CC58AB-76F2-654F-AF63-68000043A52A}">
   <dimension ref="A1:B48"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+    <sheetView topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="B48" sqref="B48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -2091,7 +2198,7 @@
         <v>94</v>
       </c>
       <c r="B47" t="s">
-        <v>298</v>
+        <v>420</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.3">
@@ -2226,7 +2333,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C900AB2-F638-4F4B-AE06-86AE70283718}">
   <dimension ref="A1:B42"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A13" workbookViewId="0">
       <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
@@ -2948,8 +3055,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57691AD4-EC7F-314E-AE2B-7AE44975FF17}">
   <dimension ref="A1:B69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="A70" sqref="A70:XFD70"/>
+    <sheetView topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="A58" sqref="A58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -3514,6 +3621,450 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C4E51FD-134B-4F7D-944E-72394CBEB357}">
+  <dimension ref="A2:B25"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="2" width="51.796875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B2" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>56</v>
+      </c>
+      <c r="B4" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>55</v>
+      </c>
+      <c r="B5" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>54</v>
+      </c>
+      <c r="B6" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>60</v>
+      </c>
+      <c r="B7" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>2</v>
+      </c>
+      <c r="B8" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>4</v>
+      </c>
+      <c r="B9" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>3</v>
+      </c>
+      <c r="B10" t="s">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>68</v>
+      </c>
+      <c r="B11" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>66</v>
+      </c>
+      <c r="B12" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>421</v>
+      </c>
+      <c r="B13" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>422</v>
+      </c>
+      <c r="B14" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>64</v>
+      </c>
+      <c r="B15" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>69</v>
+      </c>
+      <c r="B16" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>70</v>
+      </c>
+      <c r="B17" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>71</v>
+      </c>
+      <c r="B18" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>42</v>
+      </c>
+      <c r="B19" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>92</v>
+      </c>
+      <c r="B20" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>95</v>
+      </c>
+      <c r="B21" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>48</v>
+      </c>
+      <c r="B22" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>43</v>
+      </c>
+      <c r="B23" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>87</v>
+      </c>
+      <c r="B24" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>84</v>
+      </c>
+      <c r="B25" t="s">
+        <v>293</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC3BF35A-933F-4DF8-89D8-A08AE22C8198}">
+  <dimension ref="A2:B28"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="2" width="56.19921875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B2" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>56</v>
+      </c>
+      <c r="B4" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>55</v>
+      </c>
+      <c r="B5" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>54</v>
+      </c>
+      <c r="B6" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>2</v>
+      </c>
+      <c r="B7" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>3</v>
+      </c>
+      <c r="B9" t="s">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>68</v>
+      </c>
+      <c r="B10" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>66</v>
+      </c>
+      <c r="B11" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>421</v>
+      </c>
+      <c r="B12" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>439</v>
+      </c>
+      <c r="B13" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>64</v>
+      </c>
+      <c r="B14" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>440</v>
+      </c>
+      <c r="B15" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>50</v>
+      </c>
+      <c r="B16" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>52</v>
+      </c>
+      <c r="B17" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>87</v>
+      </c>
+      <c r="B18" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>43</v>
+      </c>
+      <c r="B19" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>48</v>
+      </c>
+      <c r="B20" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>95</v>
+      </c>
+      <c r="B21" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>93</v>
+      </c>
+      <c r="B22" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>441</v>
+      </c>
+      <c r="B23" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>442</v>
+      </c>
+      <c r="B24" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>443</v>
+      </c>
+      <c r="B25" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>444</v>
+      </c>
+      <c r="B26" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>437</v>
+      </c>
+      <c r="B27" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>42</v>
+      </c>
+      <c r="B28" t="s">
+        <v>436</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
   <clbl:label id="{f42aa342-8706-4288-bd11-ebb85995028c}" enabled="1" method="Standard" siteId="{72f988bf-86f1-41af-91ab-2d7cd011db47}" contentBits="0" removed="0"/>

</xml_diff>

<commit_message>
Fix up folder strategy
</commit_message>
<xml_diff>
--- a/xftomaui/NameMappings.xlsx
+++ b/xftomaui/NameMappings.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10220"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/redth/code/xf-to-maui/xftomaui/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\code\xf-to-maui\xftomaui\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00E1F048-A733-CA4F-A41D-DFEC2F08E1EA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{791A81FE-3B45-47A8-972B-E10059DF1256}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="520" windowWidth="25600" windowHeight="14020" firstSheet="2" activeTab="5" xr2:uid="{AB42A6E3-4848-A147-B598-85F847833A81}"/>
+    <workbookView xWindow="13500" yWindow="1836" windowWidth="20916" windowHeight="14664" firstSheet="2" activeTab="4" xr2:uid="{AB42A6E3-4848-A147-B598-85F847833A81}"/>
   </bookViews>
   <sheets>
     <sheet name="Maui.Essentials" sheetId="1" r:id="rId1"/>
@@ -509,33 +509,6 @@
     <t>./src/Controls/DualScreen/src/Xamarin.Forms.DualScreen</t>
   </si>
   <si>
-    <t>./src/Controls/Core/src</t>
-  </si>
-  <si>
-    <t>./src/Controls/Xaml/src</t>
-  </si>
-  <si>
-    <t>./src/Controls/Xaml.Design/src</t>
-  </si>
-  <si>
-    <t>./src/Controls/Core.Design/src</t>
-  </si>
-  <si>
-    <t>./src/Controls/Core/test</t>
-  </si>
-  <si>
-    <t>./src/Controls/CustomAttributes/test</t>
-  </si>
-  <si>
-    <t>./src/Controls/Xaml/test</t>
-  </si>
-  <si>
-    <t>./src/Handlers/src</t>
-  </si>
-  <si>
-    <t>./src/Controls/Build.Tasks/src</t>
-  </si>
-  <si>
     <t>Old Dir</t>
   </si>
   <si>
@@ -689,24 +662,6 @@
     <t>Xamarin.Forms.DualScreen.csproj</t>
   </si>
   <si>
-    <t>Handlers.UnitTests.csproj</t>
-  </si>
-  <si>
-    <t>Handlers.DeviceTests.iOS.csproj</t>
-  </si>
-  <si>
-    <t>Handlers.DeviceTests.csproj</t>
-  </si>
-  <si>
-    <t>Handlers.DeviceTests.Android.csproj</t>
-  </si>
-  <si>
-    <t>Handlers-net6.csproj</t>
-  </si>
-  <si>
-    <t>Handlers.csproj</t>
-  </si>
-  <si>
     <t>Controls.CustomAttributes.csproj</t>
   </si>
   <si>
@@ -1028,15 +983,6 @@
     <t>./src/Compatibility/Core/src/WPF</t>
   </si>
   <si>
-    <t>./src/Compatibility/Core/test/Android</t>
-  </si>
-  <si>
-    <t>./src/Compatibility/Core/test/iOS</t>
-  </si>
-  <si>
-    <t>./src/Compatibility/Core/test/UAP</t>
-  </si>
-  <si>
     <t>Xamarin.Forms.AppLinks.nuspec</t>
   </si>
   <si>
@@ -1316,9 +1262,6 @@
     <t>Microsoft.Maui.Controls.Compatibility.UAP.UnitTests</t>
   </si>
   <si>
-    <t>Microsoft.Maui.Handlers.DeviceTests</t>
-  </si>
-  <si>
     <t>XamarinEssentialsTests</t>
   </si>
   <si>
@@ -1376,15 +1319,6 @@
     <t>Microsoft.Maui.Controls.Debug.targets</t>
   </si>
   <si>
-    <t>./src/Controls/Core/samples/Maui.Controls.Sample</t>
-  </si>
-  <si>
-    <t>./src/Controls/Core/samples/Maui.Controls.Sample.Droid</t>
-  </si>
-  <si>
-    <t>./src/Controls/Core/samples/Maui.Controls.Sample.iOS</t>
-  </si>
-  <si>
     <t>./src/Forms/samples/Maui.Controls.Sample.Droid</t>
   </si>
   <si>
@@ -1397,25 +1331,91 @@
     <t>./src/Platform.Handlers/tests/Xamarin.Platform.Handlers.Benchmarks</t>
   </si>
   <si>
-    <t>./src/Handlers/tests/DeviceTests</t>
-  </si>
-  <si>
-    <t>./src/Handlers/tests/DeviceTests.Android</t>
-  </si>
-  <si>
-    <t>./src/Handlers/tests/DeviceTests.iOS</t>
-  </si>
-  <si>
-    <t>./src/Handlers/tests/Benchmarks</t>
-  </si>
-  <si>
-    <t>./src/Handlers/tests/UnitTests</t>
-  </si>
-  <si>
     <t>Xamarin.Platform.Handlers.Benchmarks.csproj</t>
   </si>
   <si>
-    <t>Handlers.Benchmarks.csproj</t>
+    <t>./src/Core/src</t>
+  </si>
+  <si>
+    <t>./src/Core/tests/DeviceTests</t>
+  </si>
+  <si>
+    <t>./src/Core/tests/DeviceTests.Android</t>
+  </si>
+  <si>
+    <t>./src/Core/tests/DeviceTests.iOS</t>
+  </si>
+  <si>
+    <t>./src/Core/tests/UnitTests</t>
+  </si>
+  <si>
+    <t>./src/Core/tests/Benchmarks</t>
+  </si>
+  <si>
+    <t>./src/Controls/src/Build.Tasks</t>
+  </si>
+  <si>
+    <t>./src/Controls/src/Core.Design</t>
+  </si>
+  <si>
+    <t>./src/Controls/src/Core</t>
+  </si>
+  <si>
+    <t>./src/Controls/src/Xaml.Design</t>
+  </si>
+  <si>
+    <t>./src/Controls/src/Xaml</t>
+  </si>
+  <si>
+    <t>Microsoft.Maui.Core.DeviceTests</t>
+  </si>
+  <si>
+    <t>Core.UnitTests.csproj</t>
+  </si>
+  <si>
+    <t>Core.DeviceTests.iOS.csproj</t>
+  </si>
+  <si>
+    <t>Core.DeviceTests.csproj</t>
+  </si>
+  <si>
+    <t>Core.DeviceTests.Android.csproj</t>
+  </si>
+  <si>
+    <t>Core-net6.csproj</t>
+  </si>
+  <si>
+    <t>Core.Benchmarks.csproj</t>
+  </si>
+  <si>
+    <t>Core.csproj</t>
+  </si>
+  <si>
+    <t>./src/Controls/samples/Maui.Controls.Sample</t>
+  </si>
+  <si>
+    <t>./src/Controls/samples/Maui.Controls.Sample.Droid</t>
+  </si>
+  <si>
+    <t>./src/Controls/samples/Maui.Controls.Sample.iOS</t>
+  </si>
+  <si>
+    <t>./src/Controls/tests/Core.UnitTests</t>
+  </si>
+  <si>
+    <t>./src/Controls/tests/CustomAttributes</t>
+  </si>
+  <si>
+    <t>./src/Controls/tests/Xaml.UnitTests</t>
+  </si>
+  <si>
+    <t>./src/Compatibility/Core/tests/Android</t>
+  </si>
+  <si>
+    <t>./src/Compatibility/Core/tests/iOS</t>
+  </si>
+  <si>
+    <t>./src/Compatibility/Core/tests/UAP</t>
   </si>
 </sst>
 </file>
@@ -1791,13 +1791,13 @@
       <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.69921875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>106</v>
       </c>
@@ -1805,7 +1805,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>95</v>
       </c>
@@ -1822,17 +1822,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4CC58AB-76F2-654F-AF63-68000043A52A}">
   <dimension ref="A1:B48"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A22" workbookViewId="0">
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="56.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="81.1640625" customWidth="1"/>
+    <col min="1" max="1" width="56.796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="81.19921875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>106</v>
       </c>
@@ -1840,380 +1840,380 @@
         <v>107</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>34</v>
       </c>
       <c r="B2" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>35</v>
       </c>
       <c r="B3" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>64</v>
       </c>
       <c r="B4" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>65</v>
       </c>
       <c r="B5" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>66</v>
       </c>
       <c r="B6" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>67</v>
       </c>
       <c r="B7" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>68</v>
       </c>
       <c r="B8" t="s">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>69</v>
       </c>
       <c r="B9" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>70</v>
       </c>
       <c r="B10" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>71</v>
       </c>
       <c r="B11" t="s">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>72</v>
       </c>
       <c r="B12" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>90</v>
       </c>
       <c r="B13" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>87</v>
       </c>
       <c r="B14" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>8</v>
       </c>
       <c r="B15" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>37</v>
       </c>
       <c r="B16" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>38</v>
       </c>
       <c r="B17" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>39</v>
       </c>
       <c r="B18" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>43</v>
       </c>
       <c r="B19" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>44</v>
       </c>
       <c r="B20" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>45</v>
       </c>
       <c r="B21" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>46</v>
       </c>
       <c r="B22" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>47</v>
       </c>
       <c r="B23" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>48</v>
       </c>
       <c r="B24" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>49</v>
       </c>
       <c r="B25" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>50</v>
       </c>
       <c r="B26" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>51</v>
       </c>
       <c r="B27" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>52</v>
       </c>
       <c r="B28" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>61</v>
       </c>
       <c r="B29" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>62</v>
       </c>
       <c r="B30" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>63</v>
       </c>
       <c r="B31" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>73</v>
       </c>
       <c r="B32" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>74</v>
       </c>
       <c r="B33" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>75</v>
       </c>
       <c r="B34" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>76</v>
       </c>
       <c r="B35" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>77</v>
       </c>
       <c r="B36" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>79</v>
       </c>
       <c r="B37" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>80</v>
       </c>
       <c r="B38" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>81</v>
       </c>
       <c r="B39" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>83</v>
       </c>
       <c r="B40" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>84</v>
       </c>
       <c r="B41" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>85</v>
       </c>
       <c r="B42" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>86</v>
       </c>
       <c r="B43" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>88</v>
       </c>
       <c r="B44" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>89</v>
       </c>
       <c r="B45" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>93</v>
       </c>
       <c r="B46" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>94</v>
       </c>
       <c r="B47" t="s">
-        <v>411</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>96</v>
       </c>
       <c r="B48" t="s">
-        <v>294</v>
+        <v>279</v>
       </c>
     </row>
   </sheetData>
@@ -2226,16 +2226,16 @@
   <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="48.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="38.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="48.19921875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="38.19921875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>106</v>
       </c>
@@ -2243,7 +2243,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -2251,7 +2251,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -2259,7 +2259,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -2267,7 +2267,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>40</v>
       </c>
@@ -2275,7 +2275,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>41</v>
       </c>
@@ -2283,7 +2283,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>42</v>
       </c>
@@ -2291,7 +2291,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>78</v>
       </c>
@@ -2299,7 +2299,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>82</v>
       </c>
@@ -2307,7 +2307,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>91</v>
       </c>
@@ -2315,7 +2315,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>92</v>
       </c>
@@ -2323,7 +2323,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>93</v>
       </c>
@@ -2340,17 +2340,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C900AB2-F638-4F4B-AE06-86AE70283718}">
   <dimension ref="A1:B42"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection sqref="A1:B1"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A46" sqref="A46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="41.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="95.6640625" customWidth="1"/>
+    <col min="1" max="1" width="41.69921875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="95.69921875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>106</v>
       </c>
@@ -2358,332 +2358,332 @@
         <v>107</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>362</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>363</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>365</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>366</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>9</v>
       </c>
       <c r="B7" t="s">
-        <v>367</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>10</v>
       </c>
       <c r="B8" t="s">
-        <v>368</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>11</v>
       </c>
       <c r="B9" t="s">
-        <v>369</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>12</v>
       </c>
       <c r="B10" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>13</v>
       </c>
       <c r="B11" t="s">
-        <v>371</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>14</v>
       </c>
       <c r="B12" t="s">
-        <v>372</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>15</v>
       </c>
       <c r="B13" t="s">
-        <v>401</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>16</v>
       </c>
       <c r="B14" t="s">
-        <v>373</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>17</v>
       </c>
       <c r="B15" t="s">
-        <v>374</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>18</v>
       </c>
       <c r="B16" t="s">
-        <v>375</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>19</v>
       </c>
       <c r="B17" t="s">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>20</v>
       </c>
       <c r="B18" t="s">
-        <v>377</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>21</v>
       </c>
       <c r="B19" t="s">
-        <v>378</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>22</v>
       </c>
       <c r="B20" t="s">
-        <v>379</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>23</v>
       </c>
       <c r="B21" t="s">
-        <v>380</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>24</v>
       </c>
       <c r="B22" t="s">
-        <v>381</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>25</v>
       </c>
       <c r="B23" t="s">
-        <v>382</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>26</v>
       </c>
       <c r="B24" t="s">
-        <v>383</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>27</v>
       </c>
       <c r="B25" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>28</v>
       </c>
       <c r="B26" t="s">
-        <v>385</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>29</v>
       </c>
       <c r="B27" t="s">
-        <v>386</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>30</v>
       </c>
       <c r="B28" t="s">
-        <v>387</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>31</v>
       </c>
       <c r="B29" t="s">
-        <v>388</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>32</v>
       </c>
       <c r="B30" t="s">
-        <v>389</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>33</v>
       </c>
       <c r="B31" t="s">
-        <v>402</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>36</v>
       </c>
       <c r="B32" t="s">
-        <v>390</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>54</v>
       </c>
       <c r="B33" t="s">
-        <v>391</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>55</v>
       </c>
       <c r="B34" t="s">
-        <v>392</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>53</v>
       </c>
       <c r="B35" t="s">
-        <v>393</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>56</v>
       </c>
       <c r="B36" t="s">
-        <v>394</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>57</v>
       </c>
       <c r="B37" t="s">
-        <v>395</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>58</v>
       </c>
       <c r="B38" t="s">
-        <v>396</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>59</v>
       </c>
       <c r="B39" t="s">
-        <v>397</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>60</v>
       </c>
       <c r="B40" t="s">
-        <v>398</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>81</v>
       </c>
       <c r="B41" t="s">
-        <v>399</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>93</v>
       </c>
       <c r="B42" t="s">
-        <v>400</v>
+        <v>382</v>
       </c>
     </row>
   </sheetData>
@@ -2695,264 +2695,264 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0873AE8A-7AB4-EC41-9198-123A3D96031C}">
   <dimension ref="A1:B46"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="B46" sqref="B46"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="2" width="68" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>163</v>
+        <v>154</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>135</v>
       </c>
       <c r="B2" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>131</v>
       </c>
       <c r="B3" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>134</v>
       </c>
       <c r="B4" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>136</v>
       </c>
       <c r="B5" t="s">
-        <v>316</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>137</v>
       </c>
       <c r="B6" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>133</v>
       </c>
       <c r="B7" t="s">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>130</v>
       </c>
       <c r="B8" t="s">
-        <v>323</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>138</v>
       </c>
       <c r="B9" t="s">
-        <v>324</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>140</v>
       </c>
       <c r="B10" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>139</v>
       </c>
       <c r="B11" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>132</v>
       </c>
       <c r="B12" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>127</v>
       </c>
       <c r="B13" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>129</v>
       </c>
       <c r="B14" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>128</v>
       </c>
       <c r="B15" t="s">
-        <v>329</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>148</v>
       </c>
       <c r="B16" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>143</v>
       </c>
       <c r="B17" t="s">
-        <v>307</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>145</v>
       </c>
       <c r="B18" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>146</v>
       </c>
       <c r="B19" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>142</v>
       </c>
       <c r="B20" t="s">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>141</v>
       </c>
       <c r="B21" t="s">
-        <v>311</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>144</v>
       </c>
       <c r="B22" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>147</v>
       </c>
       <c r="B23" t="s">
-        <v>437</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>149</v>
       </c>
       <c r="B24" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>150</v>
       </c>
       <c r="B25" t="s">
-        <v>314</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>151</v>
       </c>
       <c r="B26" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>121</v>
       </c>
       <c r="B27" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>122</v>
       </c>
       <c r="B28" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>123</v>
       </c>
       <c r="B29" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>118</v>
       </c>
       <c r="B30" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>116</v>
       </c>
       <c r="B31" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>153</v>
       </c>
@@ -2960,7 +2960,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>152</v>
       </c>
@@ -2968,55 +2968,55 @@
         <v>124</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
+        <v>426</v>
+      </c>
+      <c r="B34" t="s">
         <v>448</v>
       </c>
-      <c r="B34" t="s">
-        <v>443</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>446</v>
+        <v>424</v>
       </c>
       <c r="B35" t="s">
-        <v>444</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>447</v>
+        <v>425</v>
       </c>
       <c r="B36" t="s">
-        <v>445</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>119</v>
       </c>
       <c r="B37" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>120</v>
       </c>
       <c r="B38" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>117</v>
       </c>
       <c r="B39" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>126</v>
       </c>
@@ -3024,52 +3024,52 @@
         <v>110</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>115</v>
       </c>
       <c r="B41" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>113</v>
       </c>
       <c r="B42" t="s">
-        <v>450</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>114</v>
       </c>
       <c r="B43" t="s">
-        <v>451</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>112</v>
       </c>
       <c r="B44" t="s">
-        <v>452</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>111</v>
       </c>
       <c r="B45" t="s">
-        <v>454</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>449</v>
+        <v>427</v>
       </c>
       <c r="B46" t="s">
-        <v>453</v>
+        <v>434</v>
       </c>
     </row>
   </sheetData>
@@ -3086,573 +3086,573 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57691AD4-EC7F-314E-AE2B-7AE44975FF17}">
   <dimension ref="A1:B70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A68" workbookViewId="0">
-      <selection activeCell="B78" sqref="B78"/>
+    <sheetView topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="2" width="54" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>403</v>
+        <v>385</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>404</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>156</v>
+      </c>
+      <c r="B2" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>157</v>
+      </c>
+      <c r="B3" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>158</v>
+      </c>
+      <c r="B4" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>159</v>
+      </c>
+      <c r="B5" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>160</v>
+      </c>
+      <c r="B6" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>428</v>
+      </c>
+      <c r="B7" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>161</v>
+      </c>
+      <c r="B8" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>162</v>
+      </c>
+      <c r="B9" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>163</v>
+      </c>
+      <c r="B10" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>164</v>
+      </c>
+      <c r="B11" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
         <v>165</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B12" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>166</v>
+      </c>
+      <c r="B13" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>167</v>
+      </c>
+      <c r="B14" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>168</v>
+      </c>
+      <c r="B15" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>169</v>
+      </c>
+      <c r="B16" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>170</v>
+      </c>
+      <c r="B17" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>171</v>
+      </c>
+      <c r="B18" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>166</v>
-      </c>
-      <c r="B3" t="s">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>172</v>
+      </c>
+      <c r="B19" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>167</v>
-      </c>
-      <c r="B4" t="s">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>173</v>
+      </c>
+      <c r="B20" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>168</v>
-      </c>
-      <c r="B5" t="s">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>174</v>
+      </c>
+      <c r="B21" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>169</v>
-      </c>
-      <c r="B6" t="s">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>175</v>
+      </c>
+      <c r="B22" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>455</v>
-      </c>
-      <c r="B7" t="s">
-        <v>456</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>170</v>
-      </c>
-      <c r="B8" t="s">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>176</v>
+      </c>
+      <c r="B23" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>171</v>
-      </c>
-      <c r="B9" t="s">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>177</v>
+      </c>
+      <c r="B24" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>172</v>
-      </c>
-      <c r="B10" t="s">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>178</v>
+      </c>
+      <c r="B25" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>173</v>
-      </c>
-      <c r="B11" t="s">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>179</v>
+      </c>
+      <c r="B26" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>174</v>
-      </c>
-      <c r="B12" t="s">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>180</v>
+      </c>
+      <c r="B27" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>175</v>
-      </c>
-      <c r="B13" t="s">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>181</v>
+      </c>
+      <c r="B28" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>176</v>
-      </c>
-      <c r="B14" t="s">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>182</v>
+      </c>
+      <c r="B29" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>177</v>
-      </c>
-      <c r="B15" t="s">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>183</v>
+      </c>
+      <c r="B30" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>178</v>
-      </c>
-      <c r="B16" t="s">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>184</v>
+      </c>
+      <c r="B31" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>179</v>
-      </c>
-      <c r="B17" t="s">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>185</v>
+      </c>
+      <c r="B32" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>180</v>
-      </c>
-      <c r="B18" t="s">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>186</v>
+      </c>
+      <c r="B33" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>181</v>
-      </c>
-      <c r="B19" t="s">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>187</v>
+      </c>
+      <c r="B34" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
-        <v>182</v>
-      </c>
-      <c r="B20" t="s">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>188</v>
+      </c>
+      <c r="B35" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
-        <v>183</v>
-      </c>
-      <c r="B21" t="s">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>189</v>
+      </c>
+      <c r="B36" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
-        <v>184</v>
-      </c>
-      <c r="B22" t="s">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>190</v>
+      </c>
+      <c r="B37" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
-        <v>185</v>
-      </c>
-      <c r="B23" t="s">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>191</v>
+      </c>
+      <c r="B38" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
-        <v>186</v>
-      </c>
-      <c r="B24" t="s">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>192</v>
+      </c>
+      <c r="B39" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
-        <v>187</v>
-      </c>
-      <c r="B25" t="s">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>193</v>
+      </c>
+      <c r="B40" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
-        <v>188</v>
-      </c>
-      <c r="B26" t="s">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>194</v>
+      </c>
+      <c r="B41" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
-        <v>189</v>
-      </c>
-      <c r="B27" t="s">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>195</v>
+      </c>
+      <c r="B42" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
-        <v>190</v>
-      </c>
-      <c r="B28" t="s">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>196</v>
+      </c>
+      <c r="B43" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
-        <v>191</v>
-      </c>
-      <c r="B29" t="s">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>197</v>
+      </c>
+      <c r="B44" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A30" t="s">
-        <v>192</v>
-      </c>
-      <c r="B30" t="s">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>198</v>
+      </c>
+      <c r="B45" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A31" t="s">
-        <v>193</v>
-      </c>
-      <c r="B31" t="s">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>199</v>
+      </c>
+      <c r="B46" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A32" t="s">
-        <v>194</v>
-      </c>
-      <c r="B32" t="s">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
+        <v>200</v>
+      </c>
+      <c r="B47" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A33" t="s">
-        <v>195</v>
-      </c>
-      <c r="B33" t="s">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
+        <v>201</v>
+      </c>
+      <c r="B48" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A34" t="s">
-        <v>196</v>
-      </c>
-      <c r="B34" t="s">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
+        <v>202</v>
+      </c>
+      <c r="B49" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A35" t="s">
-        <v>197</v>
-      </c>
-      <c r="B35" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A36" t="s">
-        <v>198</v>
-      </c>
-      <c r="B36" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A37" t="s">
-        <v>199</v>
-      </c>
-      <c r="B37" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A38" t="s">
-        <v>200</v>
-      </c>
-      <c r="B38" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A39" t="s">
-        <v>201</v>
-      </c>
-      <c r="B39" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A40" t="s">
-        <v>202</v>
-      </c>
-      <c r="B40" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A41" t="s">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
         <v>203</v>
       </c>
-      <c r="B41" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A42" t="s">
+      <c r="B50" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
         <v>204</v>
       </c>
-      <c r="B42" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A43" t="s">
-        <v>205</v>
-      </c>
-      <c r="B43" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A44" t="s">
-        <v>206</v>
-      </c>
-      <c r="B44" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A45" t="s">
-        <v>207</v>
-      </c>
-      <c r="B45" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A46" t="s">
-        <v>208</v>
-      </c>
-      <c r="B46" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A47" t="s">
-        <v>209</v>
-      </c>
-      <c r="B47" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A48" t="s">
-        <v>210</v>
-      </c>
-      <c r="B48" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A49" t="s">
-        <v>211</v>
-      </c>
-      <c r="B49" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A50" t="s">
-        <v>212</v>
-      </c>
-      <c r="B50" t="s">
-        <v>360</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A51" t="s">
-        <v>213</v>
-      </c>
       <c r="B51" t="s">
-        <v>359</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
+        <v>312</v>
+      </c>
+      <c r="B52" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
+        <v>313</v>
+      </c>
+      <c r="B53" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
+        <v>314</v>
+      </c>
+      <c r="B54" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
+        <v>315</v>
+      </c>
+      <c r="B55" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A56" t="s">
+        <v>316</v>
+      </c>
+      <c r="B56" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A57" t="s">
+        <v>317</v>
+      </c>
+      <c r="B57" t="s">
         <v>330</v>
       </c>
-      <c r="B52" t="s">
-        <v>441</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A53" t="s">
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A58" t="s">
+        <v>318</v>
+      </c>
+      <c r="B58" t="s">
         <v>331</v>
       </c>
-      <c r="B53" t="s">
-        <v>442</v>
-      </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A54" t="s">
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A59" t="s">
+        <v>319</v>
+      </c>
+      <c r="B59" t="s">
         <v>332</v>
       </c>
-      <c r="B54" t="s">
-        <v>347</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A55" t="s">
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A60" t="s">
+        <v>320</v>
+      </c>
+      <c r="B60" t="s">
         <v>333</v>
       </c>
-      <c r="B55" t="s">
-        <v>346</v>
-      </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A56" t="s">
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A61" t="s">
+        <v>321</v>
+      </c>
+      <c r="B61" t="s">
         <v>334</v>
       </c>
-      <c r="B56" t="s">
-        <v>361</v>
-      </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A57" t="s">
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A62" t="s">
+        <v>322</v>
+      </c>
+      <c r="B62" t="s">
         <v>335</v>
       </c>
-      <c r="B57" t="s">
-        <v>348</v>
-      </c>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A58" t="s">
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A63" t="s">
+        <v>323</v>
+      </c>
+      <c r="B63" t="s">
         <v>336</v>
       </c>
-      <c r="B58" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A59" t="s">
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A64" t="s">
+        <v>324</v>
+      </c>
+      <c r="B64" t="s">
         <v>337</v>
       </c>
-      <c r="B59" t="s">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A60" t="s">
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A65" t="s">
+        <v>325</v>
+      </c>
+      <c r="B65" t="s">
         <v>338</v>
       </c>
-      <c r="B60" t="s">
-        <v>351</v>
-      </c>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A61" t="s">
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A66" t="s">
+        <v>326</v>
+      </c>
+      <c r="B66" t="s">
         <v>339</v>
       </c>
-      <c r="B61" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A62" t="s">
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A67" t="s">
+        <v>327</v>
+      </c>
+      <c r="B67" t="s">
         <v>340</v>
       </c>
-      <c r="B62" t="s">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A63" t="s">
-        <v>341</v>
-      </c>
-      <c r="B63" t="s">
-        <v>354</v>
-      </c>
-    </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A64" t="s">
-        <v>342</v>
-      </c>
-      <c r="B64" t="s">
-        <v>355</v>
-      </c>
-    </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A65" t="s">
-        <v>343</v>
-      </c>
-      <c r="B65" t="s">
-        <v>356</v>
-      </c>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A66" t="s">
-        <v>344</v>
-      </c>
-      <c r="B66" t="s">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A67" t="s">
-        <v>345</v>
-      </c>
-      <c r="B67" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.2">
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>405</v>
+        <v>387</v>
       </c>
       <c r="B68" t="s">
-        <v>406</v>
-      </c>
-    </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.2">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>407</v>
+        <v>389</v>
       </c>
       <c r="B69" t="s">
-        <v>408</v>
-      </c>
-    </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.2">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>409</v>
+        <v>391</v>
       </c>
       <c r="B70" t="s">
-        <v>410</v>
+        <v>392</v>
       </c>
     </row>
   </sheetData>
@@ -3665,167 +3665,167 @@
   <dimension ref="A2:B26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="51.83203125" customWidth="1"/>
+    <col min="1" max="2" width="51.796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>53</v>
       </c>
       <c r="B2" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>419</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>56</v>
       </c>
       <c r="B4" t="s">
-        <v>415</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>55</v>
       </c>
       <c r="B5" t="s">
-        <v>416</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>54</v>
       </c>
       <c r="B6" t="s">
-        <v>417</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>60</v>
       </c>
       <c r="B7" t="s">
-        <v>418</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>2</v>
       </c>
       <c r="B8" t="s">
-        <v>420</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>4</v>
       </c>
       <c r="B9" t="s">
-        <v>421</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>3</v>
       </c>
       <c r="B10" t="s">
-        <v>422</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>68</v>
       </c>
       <c r="B11" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>66</v>
       </c>
       <c r="B12" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>412</v>
+        <v>394</v>
       </c>
       <c r="B13" t="s">
-        <v>438</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>413</v>
+        <v>395</v>
       </c>
       <c r="B14" t="s">
-        <v>439</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>64</v>
       </c>
       <c r="B15" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>90</v>
       </c>
       <c r="B16" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>69</v>
       </c>
       <c r="B17" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>70</v>
       </c>
       <c r="B18" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>71</v>
       </c>
       <c r="B19" t="s">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>42</v>
       </c>
       <c r="B20" t="s">
-        <v>423</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>92</v>
       </c>
@@ -3833,7 +3833,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>95</v>
       </c>
@@ -3841,36 +3841,36 @@
         <v>98</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>48</v>
       </c>
       <c r="B23" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>43</v>
       </c>
       <c r="B24" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>87</v>
       </c>
       <c r="B25" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>84</v>
       </c>
       <c r="B26" t="s">
-        <v>289</v>
+        <v>274</v>
       </c>
     </row>
   </sheetData>
@@ -3883,175 +3883,175 @@
   <dimension ref="A2:B30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="56.1640625" customWidth="1"/>
+    <col min="1" max="2" width="56.19921875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>53</v>
       </c>
       <c r="B2" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>419</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>56</v>
       </c>
       <c r="B4" t="s">
-        <v>415</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>55</v>
       </c>
       <c r="B5" t="s">
-        <v>416</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>54</v>
       </c>
       <c r="B6" t="s">
-        <v>417</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>2</v>
       </c>
       <c r="B7" t="s">
-        <v>420</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>4</v>
       </c>
       <c r="B8" t="s">
-        <v>421</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>3</v>
       </c>
       <c r="B9" t="s">
-        <v>422</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>68</v>
       </c>
       <c r="B10" t="s">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>66</v>
       </c>
       <c r="B11" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>412</v>
+        <v>394</v>
       </c>
       <c r="B12" t="s">
-        <v>438</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>426</v>
+        <v>407</v>
       </c>
       <c r="B13" t="s">
-        <v>440</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>64</v>
       </c>
       <c r="B14" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>90</v>
       </c>
       <c r="B15" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>427</v>
+        <v>408</v>
       </c>
       <c r="B16" t="s">
-        <v>432</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>50</v>
       </c>
       <c r="B17" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>52</v>
       </c>
       <c r="B18" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>87</v>
       </c>
       <c r="B19" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>43</v>
       </c>
       <c r="B20" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>48</v>
       </c>
       <c r="B21" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>95</v>
       </c>
@@ -4059,63 +4059,63 @@
         <v>98</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>93</v>
       </c>
       <c r="B23" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>428</v>
+        <v>409</v>
       </c>
       <c r="B24" t="s">
-        <v>433</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>429</v>
+        <v>410</v>
       </c>
       <c r="B25" t="s">
-        <v>434</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>430</v>
+        <v>411</v>
       </c>
       <c r="B26" t="s">
-        <v>435</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>431</v>
+        <v>412</v>
       </c>
       <c r="B27" t="s">
-        <v>436</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>424</v>
+        <v>405</v>
       </c>
       <c r="B28" t="s">
-        <v>425</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>42</v>
       </c>
       <c r="B29" t="s">
-        <v>423</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>92</v>
       </c>
@@ -4134,7 +4134,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>